<commit_message>
Unit test for Sprint 1 for the register page
</commit_message>
<xml_diff>
--- a/Testing/Sprint 1 Tests/SR_11.2.xlsx
+++ b/Testing/Sprint 1 Tests/SR_11.2.xlsx
@@ -169,45 +169,24 @@
     <t>Test title</t>
   </si>
   <si>
-    <t>[Sub-story] Login</t>
-  </si>
-  <si>
-    <t>User is able to pass authentication successfully</t>
-  </si>
-  <si>
     <t>Pre-condition</t>
   </si>
   <si>
-    <t>Hold a valid username and password</t>
-  </si>
-  <si>
     <t>Tested by:</t>
   </si>
   <si>
-    <t>Pamela Khouri</t>
-  </si>
-  <si>
-    <t>1- Navigate to the login page</t>
-  </si>
-  <si>
     <t>2- Enter a valid username or email</t>
   </si>
   <si>
     <t>3- Enter a valid password</t>
   </si>
   <si>
-    <t>4 - Click on the login button</t>
-  </si>
-  <si>
     <t>Tested on:</t>
   </si>
   <si>
     <t>12-04-2017</t>
   </si>
   <si>
-    <t>The user is logged in and redirected to the main dashboard page</t>
-  </si>
-  <si>
     <t>Test data</t>
   </si>
   <si>
@@ -223,10 +202,31 @@
     <t>Post-condition:</t>
   </si>
   <si>
-    <t>Account details are logged in the database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user cannot log in and remains on the login page. </t>
+    <t>Brandon Goldwax</t>
+  </si>
+  <si>
+    <t>[Sub-story] Register</t>
+  </si>
+  <si>
+    <t>User is able to successfully register</t>
+  </si>
+  <si>
+    <t>1- Navigate to the register page</t>
+  </si>
+  <si>
+    <t>4 - Click on the register button</t>
+  </si>
+  <si>
+    <t>The user is registered using the inputed username/email and password then is redirected to the login page</t>
+  </si>
+  <si>
+    <t>The user cannot register if the username/email is already used</t>
+  </si>
+  <si>
+    <t>Account details are registered in the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hold a valid and unused username and password, </t>
   </si>
 </sst>
 </file>
@@ -972,7 +972,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C8" sqref="C8:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1010,13 +1010,13 @@
         <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1024,13 +1024,13 @@
         <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="13.9" x14ac:dyDescent="0.25">
@@ -1038,15 +1038,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="13.9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="13.9" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
@@ -1069,16 +1069,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="41.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="25" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>0</v>
@@ -1090,10 +1090,10 @@
     </row>
     <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="22"/>
@@ -1102,10 +1102,10 @@
     </row>
     <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="22"/>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="27"/>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>60</v>

</xml_diff>